<commit_message>
Replace empty tuple by None in pandas datframe
</commit_message>
<xml_diff>
--- a/data/Schedule_Plus_2022-03-14.xlsx
+++ b/data/Schedule_Plus_2022-03-14.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:K86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,7 +494,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>17737615</v>
+        <v>17684196</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -508,30 +508,26 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Zpravodajství z Česka i ze světa. Sport, Zelená vlna a předpověď počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>44640.00625</v>
+        <v>44642.00694444445</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>44640.00625</v>
+        <v>44642.00694444445</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>00:09:00</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:10:00</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="b">
         <v>0</v>
       </c>
@@ -541,46 +537,42 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>17737618</v>
+        <v>17684197</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Noční Radiožurnál</t>
+          <t>Dvacet minut Radiožurnálu</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství. Moderuje Adam Carda a Jiří Štefl.</t>
+          <t>Hostem je Josef Středula, předseda Českomoravské komory odborových svazů. V Česku se už zaregistrovalo přes dvě stě tisíc uprchlíků z Ukrajiny. Jak jejich příchod zasáhne sociální systém a pracovní trh? Je vláda na migrační vlnu připravena? Moderuje Vladimír Kroc.</t>
         </is>
       </c>
       <c r="G3" s="2" t="n">
-        <v>44640.04166666666</v>
+        <v>44642.025</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>44640.04166666666</v>
+        <v>44642.025</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>00:50:00</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>({'id': 5000223, 'name': 'Jiří Štefl'},)</t>
-        </is>
-      </c>
+          <t>00:26:00</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -588,46 +580,42 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>17737619</v>
+        <v>17684198</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Pro a proti</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Válka na Ukrajině oživila mezi částí politiků úvahy o obnovení základní vojenské povinnosti. Pro je i polovina z tisíce lidí oslovených před pár dny agenturou Median. Zvýšila by povinná vojna obranyschopnost země? Nebo bezpečnost státu lépe zajistí současná profesionální armáda začleněná do NATO a příslušníci Aktivních záloh? Debatovat budou předseda sněmovního výboru pro obranu, bývalý ministr obrany Lubomír Metnar z hnutí ANO a příslušník Aktivních záloh v hodnosti majora a režisér Václav Marhoul.</t>
         </is>
       </c>
       <c r="G4" s="2" t="n">
-        <v>44640.02222222222</v>
+        <v>44642.04166666666</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>44640.02222222222</v>
+        <v>44642.04166666666</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:24:00</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -635,7 +623,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>17737622</v>
+        <v>17684199</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -649,30 +637,26 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Zpravodajství z Česka i ze světa. Sport, Zelená vlna a předpověď počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G5" s="2" t="n">
-        <v>44640.04444444444</v>
+        <v>44642.04513888889</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>44640.04444444444</v>
+        <v>44642.04513888889</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>00:04:00</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:05:00</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
       <c r="K5" t="b">
         <v>0</v>
       </c>
@@ -682,44 +666,40 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>17737625</v>
+        <v>17684200</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>zpr</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Noční Radiožurnál</t>
+          <t>Zprávy v angličtině/News in English</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství. Moderuje Adam Carda a Jiří Štefl.</t>
+          <t>Pětiminutový přehled aktuálního dění v anglickém jazyce. News in English offers a concise, English-language overview of events in the Czech Republic in the areas of politics, the economy and culture.</t>
         </is>
       </c>
       <c r="G6" s="2" t="n">
-        <v>44640.08333333334</v>
+        <v>44642.04861111111</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>44640.08333333334</v>
+        <v>44642.04861111111</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>00:55:00</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>({'id': 5000223, 'name': 'Jiří Štefl'},)</t>
-        </is>
-      </c>
+          <t>00:05:00</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
       <c r="K6" t="b">
         <v>0</v>
       </c>
@@ -729,46 +709,42 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>17737626</v>
+        <v>17684201</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Jak to vidí...</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Jak se bude dál vyvíjet agrese Ruska proti Ukrajině se pokusil odhadnout politický geograf Jan Kofroň v pořadu Jak to vidí. Moderuje Zita Senková.</t>
         </is>
       </c>
       <c r="G7" s="2" t="n">
-        <v>44640.06388888889</v>
+        <v>44642.0625</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>44640.06388888889</v>
+        <v>44642.0625</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:20:00</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -776,7 +752,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>17737629</v>
+        <v>17684202</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -785,35 +761,27 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Zpravodajství z Česka i ze světa. Sport, Zelená vlna a předpověď počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" s="2" t="n">
-        <v>44640.08611111111</v>
+        <v>44642.06458333333</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>44640.08611111111</v>
+        <v>44642.06458333333</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>00:04:00</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:03:00</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
       <c r="K8" t="b">
         <v>0</v>
       </c>
@@ -823,46 +791,46 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>17737632</v>
+        <v>17684203</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Noční Radiožurnál</t>
+          <t>Osobnost Plus</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství. Moderuje Adam Carda a Jiří Štefl.</t>
+          <t>Kateřina Hrubešová, mediální odbornice, bývalá ředitelka Nadačního fondu nezávislé žurnalistiky. Mezi českými novináři rostou příkopy, uvedla žena, která se v médiích a digitálním prostředí pohybuje více než čtvrtstoletí a právě opustila post ředitelky Nadačního fondu nezávislé žurnalistiky. Je spokojena s tím, jak čeští novináři pokrývají ruskou agresi na Ukrajině? Považuje blokování některých dezinformačních webů za dobrý krok? A jak moc je podle ní důležité, že v Rusku kvůli konfliktu podávají výpovědi i novináři, kteří dříve podporovali prezidenta Putina? Moderuje Barbora Tachecí.</t>
         </is>
       </c>
       <c r="G9" s="2" t="n">
-        <v>44640.125</v>
+        <v>44642.08333333334</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>44640.125</v>
+        <v>44642.08333333334</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>00:55:00</t>
+          <t>00:27:00</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>({'id': 5000223, 'name': 'Jiří Štefl'},)</t>
+          <t>({'id': 5001039, 'name': 'Barbora Tachecí'},)</t>
         </is>
       </c>
       <c r="K9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -870,7 +838,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>17737633</v>
+        <v>17684204</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -884,30 +852,26 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G10" s="2" t="n">
-        <v>44640.10555555556</v>
+        <v>44642.08680555555</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>44640.10555555556</v>
+        <v>44642.08680555555</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:05:00</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
       <c r="K10" t="b">
         <v>0</v>
       </c>
@@ -917,46 +881,42 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>17737636</v>
+        <v>17684205</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Hovory</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Zpravodajství z Česka i ze světa. Sport, Zelená vlna a předpověď počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>"Představte si paneláky jako stavebnici Lega. Jenomže zatímco v západní Evropě měli k dispozici všechny kostičky, my jsme jich v Československu měli daleko méně. I to je důvod, proč naše sídliště vypadají, jak vypadají" - říká urbanistka a historička architektury Martina Koukalová. Prý jsou ale i výjimky, jako třeba pražské sídliště Barrandov. V Hovorech bude mluvit i o tom, že podobu měst píší velké dějiny, například rok 1968. Moderuje Naděžda Hávová.</t>
         </is>
       </c>
       <c r="G11" s="2" t="n">
-        <v>44640.12777777778</v>
+        <v>44642.10416666666</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>44640.12777777778</v>
+        <v>44642.10416666666</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>00:04:00</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:25:00</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -964,44 +924,36 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>17737639</v>
+        <v>17684206</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>zpr</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Noční Radiožurnál</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství. Moderuje Adam Carda a Jiří Štefl.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" s="2" t="n">
-        <v>44640.16666666666</v>
+        <v>44642.10625</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>44640.16666666666</v>
+        <v>44642.10625</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>00:55:00</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>({'id': 5000223, 'name': 'Jiří Štefl'},)</t>
-        </is>
-      </c>
+          <t>00:03:00</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
       <c r="K12" t="b">
         <v>0</v>
       </c>
@@ -1011,46 +963,42 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>17737640</v>
+        <v>17684207</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Názory a argumenty</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Den pohledem renomovaných komentátorů</t>
         </is>
       </c>
       <c r="G13" s="2" t="n">
-        <v>44640.14722222222</v>
+        <v>44642.12430555555</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>44640.14722222222</v>
+        <v>44642.12430555555</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:26:00</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -1058,7 +1006,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>17737643</v>
+        <v>17684208</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1072,30 +1020,26 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Zpravodajství z Česka i ze světa. Sport, Zelená vlna a předpověď počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G14" s="2" t="n">
-        <v>44640.16944444444</v>
+        <v>44642.12847222222</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>44640.16944444444</v>
+        <v>44642.12847222222</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>00:04:00</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:05:00</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr"/>
       <c r="K14" t="b">
         <v>0</v>
       </c>
@@ -1105,46 +1049,46 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>17737646</v>
+        <v>17684209</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Noční Radiožurnál</t>
+          <t>Jak to bylo doopravdy</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství. Moderuje Adam Carda a Jiří Štefl.</t>
+          <t>Jak naši společnost ovlivnil feminismus, nakolik jsou feministky odpovědné za pracovní povinnost žen. Nad tím se dnes ve vysílání ČRo-Plus zamýšlí historička Dana Musilová v pořadu Jak to bylo doopravdy. Připravila Ivana Chmel Denčevová. Režie Michal Bureš.</t>
         </is>
       </c>
       <c r="G15" s="2" t="n">
-        <v>44640.20833333334</v>
+        <v>44642.14583333334</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>44640.20833333334</v>
+        <v>44642.14583333334</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>00:55:00</t>
+          <t>00:25:00</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>({'id': 5000223, 'name': 'Jiří Štefl'},)</t>
+          <t>({'id': 5002368, 'name': 'Ivana Chmel Denčevová'},)</t>
         </is>
       </c>
       <c r="K15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -1152,7 +1096,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>17737647</v>
+        <v>17684210</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1161,35 +1105,27 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" s="2" t="n">
-        <v>44640.18888888889</v>
+        <v>44642.14791666667</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>44640.18888888889</v>
+        <v>44642.14791666667</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:03:00</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
       <c r="K16" t="b">
         <v>0</v>
       </c>
@@ -1199,46 +1135,42 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>17737650</v>
+        <v>17684211</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Podcast Vinohradská 12</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Říkejme jí třeba Tamara. Žije v Česku, její rodiče v Rusku. Ona je proti invazi, oni věří Putinovi. A slovo invaze ani vyslovit nemůžou ? kdo ví, co by se jim stalo. Silný příběh natočila reportérka ČRo Lucie Korcová. O rodině rozdělené pohledem na válku,  o Rusech, kteří se bojí, že když se své rodné zemi postaví, tak si pro ně někdo přijde. Podcast připravuje Matěj Skalický.</t>
         </is>
       </c>
       <c r="G17" s="2" t="n">
-        <v>44640.21111111111</v>
+        <v>44642.16666666666</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>44640.21111111111</v>
+        <v>44642.16666666666</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>00:04:00</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:27:00</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr"/>
       <c r="K17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1246,44 +1178,40 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>17737653</v>
+        <v>17684212</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>zpr</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Víkendový Ranní Radiožurnál</t>
+          <t>Zprávy</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství, informace z denního tisku. Moderuje Vojtěch Bidrman.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G18" s="2" t="n">
-        <v>44640.25</v>
+        <v>44642.17013888889</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>44640.25</v>
+        <v>44642.17013888889</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>00:55:00</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>({'id': 5003148, 'name': 'Vojtěch Bidrman'},)</t>
-        </is>
-      </c>
+          <t>00:05:00</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
       <c r="K18" t="b">
         <v>0</v>
       </c>
@@ -1293,46 +1221,42 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>17737654</v>
+        <v>17684213</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Dokument</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Výraznou osobností, ztělesňující maďarský odpor proti komunismu, byl kardinál Jozsef Mindszenti. V repríze pořadu Portréty ho připomenou publicisté Pavel Hlavatý a Jan Sedmidubský.</t>
         </is>
       </c>
       <c r="G19" s="2" t="n">
-        <v>44640.23090277778</v>
+        <v>44642.20833333334</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>44640.23090277778</v>
+        <v>44642.20833333334</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>00:02:30</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:55:00</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr"/>
       <c r="K19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -1340,7 +1264,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>17737657</v>
+        <v>17684214</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1354,30 +1278,26 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G20" s="2" t="n">
-        <v>44640.253125</v>
+        <v>44642.21180555555</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>44640.253125</v>
+        <v>44642.21180555555</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>00:04:30</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:05:00</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
       <c r="K20" t="b">
         <v>0</v>
       </c>
@@ -1387,46 +1307,46 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>17737660</v>
+        <v>17684215</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Víkendový Ranní Radiožurnál</t>
+          <t>Interview Plus</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství, informace z denního tisku. Moderuje Vojtěch Bidrman.</t>
+          <t>Tomáš Pojar, poradce premiéra Petra Fialy pro zahraničí a bezpečnost. Západní politici dosud odmítali vyslyšet žádosti ukrajinského prezidenta Volodymyra Zelenského o další pomoc ve válce s Ruskem. Vynucení bezletové zóny by podle nich vedlo k přímé konfrontaci NATO s ruskou armádou. Může nyní, tváří v tvář stoupající brutalitě Rusů, Západ změnit názor a vyslat na Ukrajinu vojáky? Moderuje Jan Bumba.</t>
         </is>
       </c>
       <c r="G21" s="2" t="n">
-        <v>44640.29166666666</v>
+        <v>44642.22916666666</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>44640.29166666666</v>
+        <v>44642.22916666666</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>00:54:30</t>
+          <t>00:25:00</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>({'id': 5003148, 'name': 'Vojtěch Bidrman'},)</t>
+          <t>({'id': 5000148, 'name': 'Jan Bumba'},)</t>
         </is>
       </c>
       <c r="K21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1434,46 +1354,42 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>17737661</v>
+        <v>17684216</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Názory a argumenty</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Zpravodajství z Česka i ze světa. Sport, Zelená vlna a předpověď počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Den pohledem renomovaných komentátorů</t>
         </is>
       </c>
       <c r="G22" s="2" t="n">
-        <v>44640.26111111111</v>
+        <v>44642.25</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>44640.26111111111</v>
+        <v>44642.25</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>00:01:00</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:30:00</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
       <c r="K22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -1481,7 +1397,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>17737663</v>
+        <v>17684218</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1495,30 +1411,26 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G23" s="2" t="n">
-        <v>44640.27256944445</v>
+        <v>44642.25625</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>44640.27256944445</v>
+        <v>44642.25625</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>00:02:30</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:09:00</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr"/>
       <c r="K23" t="b">
         <v>0</v>
       </c>
@@ -1528,44 +1440,40 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>17737666</v>
+        <v>17684220</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Ranní Plus</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Zpravodajství z Česka i ze světa. Sport, Zelená vlna a předpověď počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Politika, společnost, byznys, věda</t>
         </is>
       </c>
       <c r="G24" s="2" t="n">
-        <v>44640.28159722222</v>
+        <v>44642.27083333334</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>44640.28159722222</v>
+        <v>44642.27083333334</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>00:00:30</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:20:00</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr"/>
       <c r="K24" t="b">
         <v>0</v>
       </c>
@@ -1575,7 +1483,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>17737668</v>
+        <v>17684221</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1584,35 +1492,27 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" s="2" t="n">
-        <v>44640.29479166667</v>
+        <v>44642.27291666667</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>44640.29479166667</v>
+        <v>44642.27291666667</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>00:04:30</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:03:00</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr"/>
       <c r="K25" t="b">
         <v>0</v>
       </c>
@@ -1622,44 +1522,40 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>17737671</v>
+        <v>17684223</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Víkendový Ranní Radiožurnál</t>
+          <t>Ranní Plus</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství, informace z denního tisku. Moderuje Vojtěch Bidrman.</t>
+          <t>Politika, společnost, byznys, věda</t>
         </is>
       </c>
       <c r="G26" s="2" t="n">
-        <v>44640.33333333334</v>
+        <v>44642.29166666666</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>44640.33333333334</v>
+        <v>44642.29166666666</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>00:54:30</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>({'id': 5003148, 'name': 'Vojtěch Bidrman'},)</t>
-        </is>
-      </c>
+          <t>00:26:00</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr"/>
       <c r="K26" t="b">
         <v>0</v>
       </c>
@@ -1669,7 +1565,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>17737672</v>
+        <v>17684224</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1683,30 +1579,26 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Zpravodajství z Česka i ze světa. Sport, Zelená vlna a předpověď počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G27" s="2" t="n">
-        <v>44640.30277777778</v>
+        <v>44642.29791666667</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>44640.30277777778</v>
+        <v>44642.29791666667</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>00:01:00</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:09:00</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr"/>
       <c r="K27" t="b">
         <v>0</v>
       </c>
@@ -1716,44 +1608,40 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>17737674</v>
+        <v>17684226</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Ranní Plus</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Politika, společnost, byznys, věda</t>
         </is>
       </c>
       <c r="G28" s="2" t="n">
-        <v>44640.31423611111</v>
+        <v>44642.33333333334</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>44640.31423611111</v>
+        <v>44642.33333333334</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>00:02:30</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:50:00</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr"/>
       <c r="K28" t="b">
         <v>0</v>
       </c>
@@ -1763,7 +1651,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>17737677</v>
+        <v>17684227</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1772,35 +1660,27 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Zpravodajství z Česka i ze světa. Sport, Zelená vlna a předpověď počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr"/>
       <c r="G29" s="2" t="n">
-        <v>44640.32326388889</v>
+        <v>44642.31458333333</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>44640.32326388889</v>
+        <v>44642.31458333333</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>00:00:30</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:03:00</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr"/>
       <c r="K29" t="b">
         <v>0</v>
       </c>
@@ -1810,7 +1690,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>17737679</v>
+        <v>17684229</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1824,30 +1704,26 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G30" s="2" t="n">
-        <v>44640.33645833333</v>
+        <v>44642.34027777778</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>44640.33645833333</v>
+        <v>44642.34027777778</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>00:04:30</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:10:00</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr"/>
       <c r="K30" t="b">
         <v>0</v>
       </c>
@@ -1857,7 +1733,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>17737682</v>
+        <v>17684231</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1866,35 +1742,31 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Speciál Radiožurnálu: Válka na Ukrajině</t>
+          <t>Téma dne</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Moderuje Vladimír Kroc.</t>
+          <t>Rozhovor s klíčovými osobnostmi, které rozhodují o dění v politice, byznysu, kultuře, ale i v dalších důležitých oblastech naší společnosti.</t>
         </is>
       </c>
       <c r="G31" s="2" t="n">
-        <v>44640.375</v>
+        <v>44642.375</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>44640.375</v>
+        <v>44642.375</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>00:54:30</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>({'id': 5004021, 'name': 'Vladimír Kroc'},)</t>
-        </is>
-      </c>
+          <t>00:50:00</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr"/>
       <c r="K31" t="b">
         <v>0</v>
       </c>
@@ -1904,7 +1776,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>17737685</v>
+        <v>17684232</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1913,35 +1785,27 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
       <c r="G32" s="2" t="n">
-        <v>44640.35555555556</v>
+        <v>44642.35625</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>44640.35555555556</v>
+        <v>44642.35625</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:03:00</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr"/>
       <c r="K32" t="b">
         <v>0</v>
       </c>
@@ -1951,7 +1815,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>17737691</v>
+        <v>17684235</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1965,30 +1829,26 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G33" s="2" t="n">
-        <v>44640.378125</v>
+        <v>44642.38125</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>44640.378125</v>
+        <v>44642.38125</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>00:04:30</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:09:00</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr"/>
       <c r="K33" t="b">
         <v>0</v>
       </c>
@@ -1998,44 +1858,40 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>17737694</v>
+        <v>17684237</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Zápisník zahraničních zpravodajů</t>
+          <t>Ranní Plus</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Nejlepší reportáže zahraničních zpravodajů a reportérů Radiožurnálu.</t>
+          <t>Politika, společnost, byznys, věda</t>
         </is>
       </c>
       <c r="G34" s="2" t="n">
-        <v>44640.41666666666</v>
+        <v>44642.39583333334</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>44640.41666666666</v>
+        <v>44642.39583333334</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>00:53:30</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:20:00</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr"/>
       <c r="K34" t="b">
         <v>0</v>
       </c>
@@ -2045,7 +1901,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>17737695</v>
+        <v>17684238</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -2054,35 +1910,27 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr"/>
       <c r="G35" s="2" t="n">
-        <v>44640.39722222222</v>
+        <v>44642.39791666667</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>44640.39722222222</v>
+        <v>44642.39791666667</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:03:00</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr"/>
       <c r="K35" t="b">
         <v>0</v>
       </c>
@@ -2092,44 +1940,40 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>17737698</v>
+        <v>17684240</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Ranní Plus</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Politika, společnost, byznys, věda</t>
         </is>
       </c>
       <c r="G36" s="2" t="n">
-        <v>44640.41979166667</v>
+        <v>44642.41666666666</v>
       </c>
       <c r="H36" s="2" t="n">
-        <v>44640.41979166667</v>
+        <v>44642.41666666666</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>00:04:30</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:26:00</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr"/>
       <c r="K36" t="b">
         <v>0</v>
       </c>
@@ -2139,44 +1983,40 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>17737701</v>
+        <v>17684241</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>pub</t>
+          <t>zpr</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Host Radiožurnálu</t>
+          <t>Zprávy</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Zubní lékařka Gabriela Pavlíková má pověst odbornice, která také ráda poradí a zasvěceně vysvětlí situaci. 20. březen je světový den ústního zdraví. Týká se to jen zubů a dásní? Co o naší kondici vypovídají časté opary nebo třeba bolestivé afty? Moderuje Patricie Strouhalová.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G37" s="2" t="n">
-        <v>44640.45833333334</v>
+        <v>44642.42291666667</v>
       </c>
       <c r="H37" s="2" t="n">
-        <v>44640.45833333334</v>
+        <v>44642.42291666667</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>00:54:00</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>({'id': 5001072, 'name': 'Patricie Strouhalová'},)</t>
-        </is>
-      </c>
+          <t>00:09:00</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr"/>
       <c r="K37" t="b">
         <v>0</v>
       </c>
@@ -2186,42 +2026,42 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>17737702</v>
+        <v>17684243</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Pro a proti</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Před válkou už uteklo do České republiky přes 270 tisíc Ukrajinců. Bude si Česko vědět rady s jejich začleňováním do společnosti, když se naše politická reprezentace dosud přijetí migrantů z různých koutů světa převážně bránila? Debatovat budou spolupředseda Zelených Michal Berg a europoslanec KDU-ČSL Tomáš Zdechovský. Moderuje Karolína Koubová.</t>
         </is>
       </c>
       <c r="G38" s="2" t="n">
-        <v>44640.43888888889</v>
+        <v>44642.4375</v>
       </c>
       <c r="H38" s="2" t="n">
-        <v>44640.43888888889</v>
+        <v>44642.4375</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>00:02:00</t>
+          <t>00:20:00</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>({'id': 5002197, 'name': 'Karolína Koubová'},)</t>
         </is>
       </c>
       <c r="K38" t="b">
@@ -2233,7 +2073,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>17737705</v>
+        <v>17684244</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -2242,35 +2082,27 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr"/>
       <c r="G39" s="2" t="n">
-        <v>44640.46145833333</v>
+        <v>44642.43958333333</v>
       </c>
       <c r="H39" s="2" t="n">
-        <v>44640.46145833333</v>
+        <v>44642.43958333333</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>00:04:30</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:03:00</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr"/>
       <c r="K39" t="b">
         <v>0</v>
       </c>
@@ -2280,44 +2112,40 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>17737708</v>
+        <v>17684246</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Víkendový Radiožurnál</t>
+          <t>Osobnost Plus</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Aktuální reportáže, nejrychlejší zpravodajství a informace pro spotřebitele. Moderuje Patricie Strouhalová.</t>
+          <t>Jiří Padevět, spisovatel a ředitel nakladatelství Academia.</t>
         </is>
       </c>
       <c r="G40" s="2" t="n">
-        <v>44640.5</v>
+        <v>44642.45833333334</v>
       </c>
       <c r="H40" s="2" t="n">
-        <v>44640.5</v>
+        <v>44642.45833333334</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>00:54:00</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>({'id': 5001072, 'name': 'Patricie Strouhalová'},)</t>
-        </is>
-      </c>
+          <t>00:26:00</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr"/>
       <c r="K40" t="b">
         <v>0</v>
       </c>
@@ -2327,7 +2155,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>17737709</v>
+        <v>17684247</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -2341,30 +2169,26 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G41" s="2" t="n">
-        <v>44640.48055555556</v>
+        <v>44642.46458333333</v>
       </c>
       <c r="H41" s="2" t="n">
-        <v>44640.48055555556</v>
+        <v>44642.46458333333</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:09:00</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr"/>
       <c r="K41" t="b">
         <v>0</v>
       </c>
@@ -2374,46 +2198,42 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>17737712</v>
+        <v>17684249</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Hlavní zprávy</t>
+          <t>Archiv Plus</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Zpravodajský souhrn. Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Jak je armáda důležitá si v době totality uvědomovala i vládnoucí komunistická strana v Československu. A tak věnovala velkou pozornost všem aktivitám, které nějak s armádou souvisely. Jak to vypadalo v rozhlasovém vysílání, po tom v archivu pátral publicista Jan Sedmidubský. A připravil Archiv Plus.</t>
         </is>
       </c>
       <c r="G42" s="2" t="n">
-        <v>44640.50590277778</v>
+        <v>44642.47916666666</v>
       </c>
       <c r="H42" s="2" t="n">
-        <v>44640.50590277778</v>
+        <v>44642.47916666666</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>00:08:30</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:20:00</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr"/>
       <c r="K42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -2421,7 +2241,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>17737715</v>
+        <v>17684250</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -2430,35 +2250,27 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Hlavní zprávy - rozhovory a komentáře</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>O všem, co se právě děje</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr"/>
       <c r="G43" s="2" t="n">
-        <v>44640.52083333334</v>
+        <v>44642.48125</v>
       </c>
       <c r="H43" s="2" t="n">
-        <v>44640.52083333334</v>
+        <v>44642.48125</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>00:20:00</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:03:00</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr"/>
       <c r="K43" t="b">
         <v>0</v>
       </c>
@@ -2468,42 +2280,42 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>17737716</v>
+        <v>17684252</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Interview Plus</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Dominik Stroukal, hlavní ekonom platební instituce Roger. České i evropské ekonomice hrozí kvůli válce na Ukrajině a rostoucí inflaci propad do recese, upozorňuje guvernér České národní banky Jiří Rusnok. O kolik mohou české domácnosti v dohledné době zchudnout? Jak souvisí růst inflace se zdražováním pohonných hmot? Moderuje Jan Bumba.</t>
         </is>
       </c>
       <c r="G44" s="2" t="n">
-        <v>44640.52222222222</v>
+        <v>44642.49930555555</v>
       </c>
       <c r="H44" s="2" t="n">
-        <v>44640.52222222222</v>
+        <v>44642.49930555555</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>00:02:00</t>
+          <t>00:25:00</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>({'id': 5000148, 'name': 'Jan Bumba'},)</t>
         </is>
       </c>
       <c r="K44" t="b">
@@ -2515,44 +2327,36 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>17737719</v>
+        <v>17684254</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>zpr</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Víkendový Radiožurnál</t>
+          <t>Hlavní zprávy</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>Aktuální reportáže, nejrychlejší zpravodajství a informace pro spotřebitele. Moderuje Patricie Strouhalová.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr"/>
       <c r="G45" s="2" t="n">
-        <v>44640.54166666666</v>
+        <v>44642.50694444445</v>
       </c>
       <c r="H45" s="2" t="n">
-        <v>44640.54166666666</v>
+        <v>44642.50694444445</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>00:26:30</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>({'id': 5001072, 'name': 'Patricie Strouhalová'},)</t>
-        </is>
-      </c>
+          <t>00:10:00</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr"/>
       <c r="K45" t="b">
         <v>0</v>
       </c>
@@ -2562,7 +2366,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>17737720</v>
+        <v>17684255</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -2571,35 +2375,27 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Speciál Radiožurnálu a ČRoPlus: Válka na Ukrajině</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr"/>
       <c r="G46" s="2" t="n">
-        <v>44640.54479166667</v>
+        <v>44642.52083333334</v>
       </c>
       <c r="H46" s="2" t="n">
-        <v>44640.54479166667</v>
+        <v>44642.52083333334</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>00:04:30</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:20:00</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr"/>
       <c r="K46" t="b">
         <v>0</v>
       </c>
@@ -2609,44 +2405,40 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>17737723</v>
+        <v>17684259</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>zpr</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Víkendový Radiožurnál</t>
+          <t>Zprávy</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Aktuální reportáže, nejrychlejší zpravodajství a informace pro spotřebitele. Moderuje Patricie Strouhalová.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G47" s="2" t="n">
-        <v>44640.58333333334</v>
+        <v>44642.54791666667</v>
       </c>
       <c r="H47" s="2" t="n">
-        <v>44640.58333333334</v>
+        <v>44642.54791666667</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>00:54:00</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>({'id': 5001072, 'name': 'Patricie Strouhalová'},)</t>
-        </is>
-      </c>
+          <t>00:09:00</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr"/>
       <c r="K47" t="b">
         <v>0</v>
       </c>
@@ -2656,46 +2448,42 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>17737724</v>
+        <v>17684258</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Jak to vidí...</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Pohledy známých osobností na věci kolem nás.</t>
         </is>
       </c>
       <c r="G48" s="2" t="n">
-        <v>44640.56388888889</v>
+        <v>44642.5625</v>
       </c>
       <c r="H48" s="2" t="n">
-        <v>44640.56388888889</v>
+        <v>44642.5625</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:20:00</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr"/>
       <c r="K48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -2703,7 +2491,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>17737727</v>
+        <v>17684262</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -2712,35 +2500,27 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr"/>
       <c r="G49" s="2" t="n">
-        <v>44640.58645833333</v>
+        <v>44642.56458333333</v>
       </c>
       <c r="H49" s="2" t="n">
-        <v>44640.58645833333</v>
+        <v>44642.56458333333</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>00:04:30</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:03:00</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr"/>
       <c r="K49" t="b">
         <v>0</v>
       </c>
@@ -2750,44 +2530,40 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>17737730</v>
+        <v>17684264</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Víkendový Radiožurnál</t>
+          <t>Názory a argumenty</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství. Moderuje Patricie Strouhalová.</t>
+          <t>Den pohledem renomovaných komentátorů</t>
         </is>
       </c>
       <c r="G50" s="2" t="n">
-        <v>44640.625</v>
+        <v>44642.58333333334</v>
       </c>
       <c r="H50" s="2" t="n">
-        <v>44640.625</v>
+        <v>44642.58333333334</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>00:54:00</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>({'id': 5001072, 'name': 'Patricie Strouhalová'},)</t>
-        </is>
-      </c>
+          <t>00:26:00</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr"/>
       <c r="K50" t="b">
         <v>0</v>
       </c>
@@ -2797,7 +2573,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>17737731</v>
+        <v>17684265</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -2811,30 +2587,26 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G51" s="2" t="n">
-        <v>44640.60555555556</v>
+        <v>44642.58958333333</v>
       </c>
       <c r="H51" s="2" t="n">
-        <v>44640.60555555556</v>
+        <v>44642.58958333333</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:09:00</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr"/>
       <c r="K51" t="b">
         <v>0</v>
       </c>
@@ -2844,44 +2616,40 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>17737734</v>
+        <v>17684267</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Odpolední Plus</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Nejnovější události v rozhovorech a reportážích</t>
         </is>
       </c>
       <c r="G52" s="2" t="n">
-        <v>44640.628125</v>
+        <v>44642.60416666666</v>
       </c>
       <c r="H52" s="2" t="n">
-        <v>44640.628125</v>
+        <v>44642.60416666666</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>00:04:30</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:20:00</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr"/>
       <c r="K52" t="b">
         <v>0</v>
       </c>
@@ -2891,44 +2659,36 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>17737737</v>
+        <v>17684268</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>zpr</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Víkendový Radiožurnál</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství. Moderuje Patricie Strouhalová.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr"/>
       <c r="G53" s="2" t="n">
-        <v>44640.66666666666</v>
+        <v>44642.60555555556</v>
       </c>
       <c r="H53" s="2" t="n">
-        <v>44640.66666666666</v>
+        <v>44642.60555555556</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>00:54:00</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>({'id': 5001072, 'name': 'Patricie Strouhalová'},)</t>
-        </is>
-      </c>
+          <t>00:02:00</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr"/>
       <c r="K53" t="b">
         <v>0</v>
       </c>
@@ -2938,46 +2698,42 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>17737738</v>
+        <v>17684270</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Podcast Vinohradská 12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Zpravodajský podcast Českého rozhlasu. Každý všední den jedno aktuální téma v souvislostech.</t>
         </is>
       </c>
       <c r="G54" s="2" t="n">
-        <v>44640.64722222222</v>
+        <v>44642.625</v>
       </c>
       <c r="H54" s="2" t="n">
-        <v>44640.64722222222</v>
+        <v>44642.625</v>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:27:00</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr"/>
       <c r="K54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -2985,7 +2741,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>17737741</v>
+        <v>17684271</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -2999,30 +2755,26 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G55" s="2" t="n">
-        <v>44640.66979166667</v>
+        <v>44642.63125</v>
       </c>
       <c r="H55" s="2" t="n">
-        <v>44640.66979166667</v>
+        <v>44642.63125</v>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>00:04:30</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:09:00</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr"/>
       <c r="K55" t="b">
         <v>0</v>
       </c>
@@ -3032,44 +2784,40 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>17737744</v>
+        <v>17684273</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Víkendový Radiožurnál</t>
+          <t>Odpolední Plus</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství. Moderuje Michaela van Erne.</t>
+          <t>Nejnovější události v rozhovorech a reportážích</t>
         </is>
       </c>
       <c r="G56" s="2" t="n">
-        <v>44640.70833333334</v>
+        <v>44642.66666666666</v>
       </c>
       <c r="H56" s="2" t="n">
-        <v>44640.70833333334</v>
+        <v>44642.66666666666</v>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>00:54:00</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>({'id': 5003523, 'name': 'Michaela van Erne'},)</t>
-        </is>
-      </c>
+          <t>00:50:00</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr"/>
       <c r="K56" t="b">
         <v>0</v>
       </c>
@@ -3079,7 +2827,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>17737745</v>
+        <v>17684274</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -3088,35 +2836,27 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr"/>
       <c r="G57" s="2" t="n">
-        <v>44640.68888888889</v>
+        <v>44642.64722222222</v>
       </c>
       <c r="H57" s="2" t="n">
-        <v>44640.68888888889</v>
+        <v>44642.64722222222</v>
       </c>
       <c r="I57" t="inlineStr">
         <is>
           <t>00:02:00</t>
         </is>
       </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+      <c r="J57" t="inlineStr"/>
       <c r="K57" t="b">
         <v>0</v>
       </c>
@@ -3126,7 +2866,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>17737748</v>
+        <v>17684276</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -3140,30 +2880,26 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Aktuální události doma i ve světě</t>
         </is>
       </c>
       <c r="G58" s="2" t="n">
-        <v>44640.71145833333</v>
+        <v>44642.67291666667</v>
       </c>
       <c r="H58" s="2" t="n">
-        <v>44640.71145833333</v>
+        <v>44642.67291666667</v>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>00:04:30</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:09:00</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr"/>
       <c r="K58" t="b">
         <v>0</v>
       </c>
@@ -3173,44 +2909,40 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>17737751</v>
+        <v>17684278</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Víkendový Radiožurnál</t>
+          <t>Odpolední Plus</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství. Moderuje Michaela van Erne.</t>
+          <t>Nejnovější události v rozhovorech a reportážích</t>
         </is>
       </c>
       <c r="G59" s="2" t="n">
-        <v>44640.75</v>
+        <v>44642.6875</v>
       </c>
       <c r="H59" s="2" t="n">
-        <v>44640.75</v>
+        <v>44642.6875</v>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>00:54:00</t>
-        </is>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>({'id': 5003523, 'name': 'Michaela van Erne'},)</t>
-        </is>
-      </c>
+          <t>00:20:00</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr"/>
       <c r="K59" t="b">
         <v>0</v>
       </c>
@@ -3220,7 +2952,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>17737752</v>
+        <v>17684279</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -3229,35 +2961,27 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr"/>
       <c r="G60" s="2" t="n">
-        <v>44640.73055555556</v>
+        <v>44642.68958333333</v>
       </c>
       <c r="H60" s="2" t="n">
-        <v>44640.73055555556</v>
+        <v>44642.68958333333</v>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:03:00</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr"/>
       <c r="K60" t="b">
         <v>0</v>
       </c>
@@ -3267,46 +2991,46 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>17737755</v>
+        <v>17684281</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Hlavní zprávy</t>
+          <t>Interview Plus</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Zpravodajský souhrn nejdůležitějších událostí dne. Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Dominik Stroukal, hlavní ekonom platební instituce Roger. České i evropské ekonomice hrozí kvůli válce na Ukrajině a rostoucí inflaci propad do recese, upozorňuje guvernér České národní banky Jiří Rusnok. O kolik mohou české domácnosti v dohledné době zchudnout? Jak souvisí růst inflace se zdražováním pohonných hmot? Moderuje Jan Bumba.</t>
         </is>
       </c>
       <c r="G61" s="2" t="n">
-        <v>44640.75694444445</v>
+        <v>44642.70763888889</v>
       </c>
       <c r="H61" s="2" t="n">
-        <v>44640.75694444445</v>
+        <v>44642.70763888889</v>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>00:10:00</t>
+          <t>00:25:00</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>({'id': 5000148, 'name': 'Jan Bumba'},)</t>
         </is>
       </c>
       <c r="K61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -3314,44 +3038,36 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>17737758</v>
+        <v>17684282</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>zpr</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Víkendový Radiožurnál</t>
+          <t>Zprávy</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství. Moderuje Michaela van Erne.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr"/>
       <c r="G62" s="2" t="n">
-        <v>44640.79166666666</v>
+        <v>44642.7125</v>
       </c>
       <c r="H62" s="2" t="n">
-        <v>44640.79166666666</v>
+        <v>44642.7125</v>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>00:49:01</t>
-        </is>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>({'id': 5003523, 'name': 'Michaela van Erne'},)</t>
-        </is>
-      </c>
+          <t>00:06:00</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr"/>
       <c r="K62" t="b">
         <v>0</v>
       </c>
@@ -3361,44 +3077,36 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>17737759</v>
+        <v>17684283</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Dvacet minut Radiožurnálu</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr"/>
       <c r="G63" s="2" t="n">
-        <v>44640.77222222222</v>
+        <v>44642.72916666666</v>
       </c>
       <c r="H63" s="2" t="n">
-        <v>44640.77222222222</v>
+        <v>44642.72916666666</v>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:24:00</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr"/>
       <c r="K63" t="b">
         <v>0</v>
       </c>
@@ -3408,7 +3116,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>17737762</v>
+        <v>17684284</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -3417,35 +3125,27 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr"/>
       <c r="G64" s="2" t="n">
-        <v>44640.79479166667</v>
+        <v>44642.73055555556</v>
       </c>
       <c r="H64" s="2" t="n">
-        <v>44640.79479166667</v>
+        <v>44642.73055555556</v>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>00:04:30</t>
-        </is>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:02:00</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr"/>
       <c r="K64" t="b">
         <v>0</v>
       </c>
@@ -3455,44 +3155,40 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>17737765</v>
+        <v>17684286</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Víkendový Radiožurnál</t>
+          <t>Odpolední Plus</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství. Moderuje Michaela van Erne.</t>
+          <t>Nejnovější události v rozhovorech a reportážích</t>
         </is>
       </c>
       <c r="G65" s="2" t="n">
-        <v>44640.83333333334</v>
+        <v>44642.75</v>
       </c>
       <c r="H65" s="2" t="n">
-        <v>44640.83333333334</v>
+        <v>44642.75</v>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>00:54:00</t>
-        </is>
-      </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>({'id': 5003523, 'name': 'Michaela van Erne'},)</t>
-        </is>
-      </c>
+          <t>00:27:00</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr"/>
       <c r="K65" t="b">
         <v>0</v>
       </c>
@@ -3502,7 +3198,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>17737766</v>
+        <v>17684287</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -3511,35 +3207,27 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Hlavní zprávy</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr"/>
       <c r="G66" s="2" t="n">
-        <v>44640.81388888889</v>
+        <v>44642.75694444445</v>
       </c>
       <c r="H66" s="2" t="n">
-        <v>44640.81388888889</v>
+        <v>44642.75694444445</v>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:10:00</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr"/>
       <c r="K66" t="b">
         <v>0</v>
       </c>
@@ -3549,7 +3237,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>17737769</v>
+        <v>17684288</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -3558,35 +3246,27 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Hlavní zprávy - rozhovory, komentáře</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr"/>
       <c r="G67" s="2" t="n">
-        <v>44640.83611111111</v>
+        <v>44642.77083333334</v>
       </c>
       <c r="H67" s="2" t="n">
-        <v>44640.83611111111</v>
+        <v>44642.77083333334</v>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>00:04:00</t>
-        </is>
-      </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:20:00</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr"/>
       <c r="K67" t="b">
         <v>0</v>
       </c>
@@ -3596,40 +3276,36 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>17737772</v>
+        <v>17684289</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>pub</t>
+          <t>zpr</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Stretnutie</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F68" t="inlineStr"/>
       <c r="G68" s="2" t="n">
-        <v>44640.85416666666</v>
+        <v>44642.77291666667</v>
       </c>
       <c r="H68" s="2" t="n">
-        <v>44640.85416666666</v>
+        <v>44642.77291666667</v>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>00:25:00</t>
-        </is>
-      </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:03:00</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr"/>
       <c r="K68" t="b">
         <v>0</v>
       </c>
@@ -3639,46 +3315,42 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>17737773</v>
+        <v>17684290</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Názory a argumenty</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Den pohledem renomovaných komentátorů</t>
         </is>
       </c>
       <c r="G69" s="2" t="n">
-        <v>44640.85555555556</v>
+        <v>44642.79166666666</v>
       </c>
       <c r="H69" s="2" t="n">
-        <v>44640.85555555556</v>
+        <v>44642.79166666666</v>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:27:00</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr"/>
       <c r="K69" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -3686,44 +3358,36 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>17737776</v>
+        <v>17684291</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>zpr</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Víkendový Radiožurnál</t>
+          <t>Zprávy</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství. Moderuje Michaela van Erne.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr"/>
       <c r="G70" s="2" t="n">
-        <v>44640.875</v>
+        <v>44642.79513888889</v>
       </c>
       <c r="H70" s="2" t="n">
-        <v>44640.875</v>
+        <v>44642.79513888889</v>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>00:27:00</t>
-        </is>
-      </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>({'id': 5003523, 'name': 'Michaela van Erne'},)</t>
-        </is>
-      </c>
+          <t>00:05:00</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr"/>
       <c r="K70" t="b">
         <v>0</v>
       </c>
@@ -3733,46 +3397,46 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>17737777</v>
+        <v>17684292</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Pro a proti</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Před válkou už uteklo do České republiky přes 270 tisíc Ukrajinců. Bude si Česko vědět rady s jejich začleňováním do společnosti, když se naše politická reprezentace dosud přijetí migrantů z různých koutů světa převážně bránila? Debatovat budou spolupředseda Zelených Michal Berg a europoslanec KDU-ČSL Tomáš Zdechovský. Moderuje Karolína Koubová.</t>
         </is>
       </c>
       <c r="G71" s="2" t="n">
-        <v>44640.87769675926</v>
+        <v>44642.8125</v>
       </c>
       <c r="H71" s="2" t="n">
-        <v>44640.87769675926</v>
+        <v>44642.8125</v>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>00:03:53</t>
+          <t>00:25:00</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>()</t>
+          <t>({'id': 5002197, 'name': 'Karolína Koubová'},)</t>
         </is>
       </c>
       <c r="K71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -3780,7 +3444,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>17737780</v>
+        <v>17684293</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -3789,31 +3453,27 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Sportžurnál</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F72" t="inlineStr"/>
       <c r="G72" s="2" t="n">
-        <v>44640.91621527778</v>
+        <v>44642.81527777778</v>
       </c>
       <c r="H72" s="2" t="n">
-        <v>44640.91621527778</v>
+        <v>44642.81527777778</v>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>00:53:55</t>
-        </is>
-      </c>
-      <c r="J72" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:04:00</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr"/>
       <c r="K72" t="b">
         <v>0</v>
       </c>
@@ -3823,46 +3483,42 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>17737781</v>
+        <v>17684294</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Osobnost Plus</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Jiří Padevět, spisovatel a ředitel nakladatelství Academia.</t>
         </is>
       </c>
       <c r="G73" s="2" t="n">
-        <v>44640.89741898148</v>
+        <v>44642.83333333334</v>
       </c>
       <c r="H73" s="2" t="n">
-        <v>44640.89741898148</v>
+        <v>44642.83333333334</v>
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>00:02:17</t>
-        </is>
-      </c>
-      <c r="J73" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:26:00</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr"/>
       <c r="K73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -3870,7 +3526,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>17737784</v>
+        <v>17684295</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -3884,30 +3540,22 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>Zpravodajství z Česka i ze světa. Sport, Zelená vlna a předpověď počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr"/>
       <c r="G74" s="2" t="n">
-        <v>44640.91944444444</v>
+        <v>44642.83680555555</v>
       </c>
       <c r="H74" s="2" t="n">
-        <v>44640.91944444444</v>
+        <v>44642.83680555555</v>
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>00:04:00</t>
-        </is>
-      </c>
-      <c r="J74" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:05:00</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr"/>
       <c r="K74" t="b">
         <v>0</v>
       </c>
@@ -3917,42 +3565,42 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>17737787</v>
+        <v>17684296</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Víkendový Radiožurnál</t>
+          <t>Ex libris</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Aktuální reportáže a nejrychlejší zpravodajství. Moderuje Michaela van Erne.</t>
+          <t>Literární magazín Ex libris v další premiéře uvede knihu Lubomíra Kopečka: Hodný zlý a ošklivý. Havel, Klaus a Zeman. Paralelní životopisy tří nejvýraznějších polistopadových politiků přečetl Libor Dvořák.</t>
         </is>
       </c>
       <c r="G75" s="2" t="n">
-        <v>44640.95833333334</v>
+        <v>44642.85416666666</v>
       </c>
       <c r="H75" s="2" t="n">
-        <v>44640.95833333334</v>
+        <v>44642.85416666666</v>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>00:55:00</t>
+          <t>00:25:00</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>({'id': 5003523, 'name': 'Michaela van Erne'},)</t>
+          <t>({'id': 5003286, 'name': 'Libor Dvořák'},)</t>
         </is>
       </c>
       <c r="K75" t="b">
@@ -3964,7 +3612,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>17737788</v>
+        <v>17684297</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -3973,35 +3621,27 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Zprávy v půl</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr"/>
       <c r="G76" s="2" t="n">
-        <v>44640.93888888889</v>
+        <v>44642.85694444444</v>
       </c>
       <c r="H76" s="2" t="n">
-        <v>44640.93888888889</v>
+        <v>44642.85694444444</v>
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J76" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:04:00</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr"/>
       <c r="K76" t="b">
         <v>0</v>
       </c>
@@ -4011,46 +3651,42 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>17737791</v>
+        <v>17684298</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Zprávy</t>
+          <t>Jak to vidí...</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Zpravodajství z Česka i ze světa. Sport, Zelená vlna a předpověď počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
+          <t>Pohledy známých osobností na věci kolem nás.</t>
         </is>
       </c>
       <c r="G77" s="2" t="n">
-        <v>44640.96111111111</v>
+        <v>44642.875</v>
       </c>
       <c r="H77" s="2" t="n">
-        <v>44640.96111111111</v>
+        <v>44642.875</v>
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>00:04:00</t>
-        </is>
-      </c>
-      <c r="J77" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
+          <t>00:26:00</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr"/>
       <c r="K77" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -4058,44 +3694,36 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>17737794</v>
+        <v>17684299</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>mag</t>
+          <t>zpr</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Host Radiožurnálu</t>
+          <t>Zprávy</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>Zubní lékařka Gabriela Pavlíková má pověst odbornice, která také ráda poradí a zasvěceně vysvětlí situaci. 20. březen je světový den ústního zdraví. Týká se to jen zubů a dásní? Co o naší kondici vypovídají časté opary nebo třeba bolestivé afty? Moderuje Patricie Strouhalová. (repríza)</t>
-        </is>
-      </c>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr"/>
       <c r="G78" s="2" t="n">
-        <v>44641</v>
+        <v>44642.88194444445</v>
       </c>
       <c r="H78" s="2" t="n">
-        <v>44641</v>
+        <v>44642.88194444445</v>
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>00:55:00</t>
-        </is>
-      </c>
-      <c r="J78" t="inlineStr">
-        <is>
-          <t>({'id': 5001072, 'name': 'Patricie Strouhalová'},)</t>
-        </is>
-      </c>
+          <t>00:10:00</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr"/>
       <c r="K78" t="b">
         <v>0</v>
       </c>
@@ -4105,46 +3733,335 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>17737795</v>
+        <v>17684300</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>zpr</t>
+          <t>pub</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
+          <t>Dokument</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Ladislav Čerych byl jeden ze světově uznávaných odborníků v oblasti sociologie a problematiky evropské spolupráce. Rodák z Čech se proslavil až v exilu, kam odešel po únoru 1948. Jeho životní příběh zpracoval do dvoudílného pořadu z cyklu Pamětníci redaktor Milan Hanuš.</t>
+        </is>
+      </c>
+      <c r="G79" s="2" t="n">
+        <v>44642.91666666666</v>
+      </c>
+      <c r="H79" s="2" t="n">
+        <v>44642.91666666666</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>00:50:00</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr"/>
+      <c r="K79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="n">
+        <v>17684301</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>zpr</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
           <t>Zprávy</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>radiozurnal</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>Z domova i ze světa. Sport, Zelená vlna a počasí. O dopravní situaci informujte na bezplatné lince 800 553 553.</t>
-        </is>
-      </c>
-      <c r="G79" s="2" t="n">
-        <v>44640.98055555556</v>
-      </c>
-      <c r="H79" s="2" t="n">
-        <v>44640.98055555556</v>
-      </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>00:02:00</t>
-        </is>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>()</t>
-        </is>
-      </c>
-      <c r="K79" t="b">
-        <v>0</v>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" s="2" t="n">
+        <v>44642.92013888889</v>
+      </c>
+      <c r="H80" s="2" t="n">
+        <v>44642.92013888889</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>00:05:00</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr"/>
+      <c r="K80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="n">
+        <v>17684302</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>pub</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Hovory</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Hostem Hovorů je filmařka Diana Cam Van Nguyen. Narodila se v Chebu, vystudovala animovaný film na pražské FAMU a její snímky se nevyhýbají vážným osobním tématům. Jedním z nich je vztah mezi generacemi v rodinách českých Vietnamců. O tomto vztahu vypráví její film Milý tati, za kterého získala Českého lva. Moderuje Petr Vizina.</t>
+        </is>
+      </c>
+      <c r="G81" s="2" t="n">
+        <v>44642.9375</v>
+      </c>
+      <c r="H81" s="2" t="n">
+        <v>44642.9375</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>00:25:00</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr"/>
+      <c r="K81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="n">
+        <v>17684303</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>zpr</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Zprávy v angličtině/News in English</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Pětiminutový přehled aktuálního dění v anglickém jazyce. News in English offers a concise, English-language overview of events in the Czech Republic in the areas of politics, the economy and culture.</t>
+        </is>
+      </c>
+      <c r="G82" s="2" t="n">
+        <v>44642.94097222222</v>
+      </c>
+      <c r="H82" s="2" t="n">
+        <v>44642.94097222222</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>00:05:00</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr"/>
+      <c r="K82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="n">
+        <v>17684304</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>pub</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Podcast Vinohradská 12</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Zpravodajský podcast Českého rozhlasu. Každý všední den jedno aktuální téma v souvislostech.</t>
+        </is>
+      </c>
+      <c r="G83" s="2" t="n">
+        <v>44642.95833333334</v>
+      </c>
+      <c r="H83" s="2" t="n">
+        <v>44642.95833333334</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>00:25:00</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr"/>
+      <c r="K83" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="n">
+        <v>17684305</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>zpr</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Zprávy</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" s="2" t="n">
+        <v>44642.96111111111</v>
+      </c>
+      <c r="H84" s="2" t="n">
+        <v>44642.96111111111</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>00:04:00</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr"/>
+      <c r="K84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="n">
+        <v>17684306</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>pub</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Názory a argumenty</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Den pohledem renomovaných komentátorů</t>
+        </is>
+      </c>
+      <c r="G85" s="2" t="n">
+        <v>44642.97916666666</v>
+      </c>
+      <c r="H85" s="2" t="n">
+        <v>44642.97916666666</v>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>00:26:00</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr"/>
+      <c r="K85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="n">
+        <v>17684307</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>pro</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Radiokniha</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>plus</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Dušan Jeřábek: Brno - kulturní město předválečné a válečné (5/10) Páté vyprávění začíná o prázdninách roku 1938, kdy autor jako student gymnázia odjíždí do tehdejší Jugoslávie. I za hranicemi Československa jsou zřejmé obavy z Hitlera, v dovolenkovém ráji se ale nesmí kritika říkat nahlas. Po návštěvě starobylého Dubrovníku a orientálního Sarajeva se studenti vrací do nervózní vlasti, kterou čeká mobilizace a následná potupa v podobě Mnichovské dohody. Obavy postihují i Brno, jehož hospody zejí prázdnotou. Všechny zasáhne smrt Karla Čapka, která je vnímána jako konec jedné éry a začátek nové smutné epochy. Tu ještě více podpoří březnová nacistická okupace, která znamená propouštění neárijských zaměstnanců. Autor popisuje setkání s budoucím básníkem Ivanem Blatným, zároveň však ztrácí svůj idol ? Arneho Nováka. V režii Zdeňka Kozáka čte Ladislav Lakomý.</t>
+        </is>
+      </c>
+      <c r="G86" s="2" t="n">
+        <v>44642.99930555555</v>
+      </c>
+      <c r="H86" s="2" t="n">
+        <v>44642.99930555555</v>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>00:26:00</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr"/>
+      <c r="K86" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>